<commit_message>
New tables for my program
</commit_message>
<xml_diff>
--- a/disk-archive-data/xls/books_razdely.xlsx
+++ b/disk-archive-data/xls/books_razdely.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>художественная литература</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Детские книги</t>
   </si>
   <si>
-    <t>х</t>
-  </si>
-  <si>
     <t xml:space="preserve">Детям 4-6 лет </t>
   </si>
   <si>
@@ -94,13 +91,73 @@
   </si>
   <si>
     <t>Детям от 12 лет</t>
+  </si>
+  <si>
+    <t>художествення литература авторов нашего времени</t>
+  </si>
+  <si>
+    <t>художественная литература авторов советского периода</t>
+  </si>
+  <si>
+    <t>Романы о любви авторов всех периодов</t>
+  </si>
+  <si>
+    <t>Романы основаны на исторических событиях</t>
+  </si>
+  <si>
+    <t>Приключенческие романы всех авторов</t>
+  </si>
+  <si>
+    <t>Ужасы, книги страшилки</t>
+  </si>
+  <si>
+    <t>книги о факторах, которые не встречается или невозможены в реальном мире</t>
+  </si>
+  <si>
+    <t>Классические произведения  зарубежных авторов</t>
+  </si>
+  <si>
+    <t>Классические произведения  русских авторов</t>
+  </si>
+  <si>
+    <t>Книги о приготовлении еды</t>
+  </si>
+  <si>
+    <t>Полезные советы в хозяйстве</t>
+  </si>
+  <si>
+    <t>Книги о здоровье человека</t>
+  </si>
+  <si>
+    <t>Советы о поделках своими руками</t>
+  </si>
+  <si>
+    <t>Книги о хобби</t>
+  </si>
+  <si>
+    <t>Книги по психологии</t>
+  </si>
+  <si>
+    <t>Исторические книги</t>
+  </si>
+  <si>
+    <t>Книги о тайнах и загадках вселенной</t>
+  </si>
+  <si>
+    <t>Учебная и нацчно популярная литература</t>
+  </si>
+  <si>
+    <t>развивающие книги, расскраски детям</t>
+  </si>
+  <si>
+    <t>Художественная и развивающая литература</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +169,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -138,9 +202,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -442,144 +507,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>